<commit_message>
Creat DB -> Product Table
</commit_message>
<xml_diff>
--- a/datacollection/project.xlsx
+++ b/datacollection/project.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hassan Ali\Desktop\newprojectsw2\Pharmacy\datacollection\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="8520" tabRatio="685"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="18192" windowHeight="8520" tabRatio="685"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="222">
   <si>
     <t>Trade Name</t>
   </si>
@@ -378,9 +383,6 @@
     <t>Penicillins.Penicillin With B-lactamase Inhibitor</t>
   </si>
   <si>
-    <t>Epicephin 1GM I.M VIAL</t>
-  </si>
-  <si>
     <t>Ceftriaxone</t>
   </si>
   <si>
@@ -667,6 +669,24 @@
   </si>
   <si>
     <t>Calcium With Vitamin C</t>
+  </si>
+  <si>
+    <t>كببببببببسسسسووووووووووولللللللللل</t>
+  </si>
+  <si>
+    <t>شششششششششششششششششششششششرب</t>
+  </si>
+  <si>
+    <t>امبول</t>
+  </si>
+  <si>
+    <t>لبوووووووس</t>
+  </si>
+  <si>
+    <t>Epicephin 1GM I.M VIAL  حقن مضادة</t>
+  </si>
+  <si>
+    <t>فوارررررررررررررررر</t>
   </si>
 </sst>
 </file>
@@ -677,7 +697,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -715,12 +735,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="نسق Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -762,7 +785,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,7 +820,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1008,21 +1031,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.375" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
-    <col min="3" max="3" width="34.875" customWidth="1"/>
-    <col min="4" max="4" width="45.75" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="4" max="4" width="45.77734375" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1056,7 +1079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1096,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1090,7 +1113,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1107,7 +1130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1124,7 +1147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1164,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1158,7 +1181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1175,7 +1198,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1192,7 +1215,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1209,7 +1232,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1226,7 +1254,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -1243,7 +1271,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1260,7 +1288,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1277,7 +1305,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1294,7 +1322,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -1311,7 +1339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -1328,7 +1356,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1345,7 +1373,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1362,7 +1390,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -1379,7 +1407,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1396,7 +1429,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1413,7 +1446,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -1430,7 +1463,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -1447,7 +1480,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1464,7 +1497,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -1481,7 +1514,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>108</v>
       </c>
@@ -1498,7 +1531,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -1515,7 +1548,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -1532,7 +1565,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -1549,32 +1582,32 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>220</v>
+      </c>
+      <c r="B34" t="s">
         <v>120</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>121</v>
-      </c>
-      <c r="C34" t="s">
-        <v>122</v>
       </c>
       <c r="D34">
         <v>36</v>
       </c>
       <c r="E34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>124</v>
       </c>
-      <c r="B35" t="s">
-        <v>125</v>
-      </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D35">
         <v>12.75</v>
@@ -1583,46 +1616,46 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" t="s">
         <v>126</v>
-      </c>
-      <c r="B36" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" t="s">
-        <v>127</v>
       </c>
       <c r="D36">
         <v>52.25</v>
       </c>
       <c r="E36" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" t="s">
         <v>128</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" t="s">
-        <v>129</v>
       </c>
       <c r="D37">
         <v>20.75</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
         <v>130</v>
-      </c>
-      <c r="B38" t="s">
-        <v>131</v>
       </c>
       <c r="C38" t="s">
         <v>80</v>
@@ -1631,117 +1664,122 @@
         <v>22.5</v>
       </c>
       <c r="E38" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
         <v>132</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>133</v>
-      </c>
-      <c r="C39" t="s">
-        <v>134</v>
       </c>
       <c r="D39">
         <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" t="s">
         <v>135</v>
-      </c>
-      <c r="B40" t="s">
-        <v>131</v>
-      </c>
-      <c r="C40" t="s">
-        <v>136</v>
       </c>
       <c r="D40">
         <v>47</v>
       </c>
       <c r="E40" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" t="s">
         <v>137</v>
-      </c>
-      <c r="B41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" t="s">
-        <v>138</v>
       </c>
       <c r="D41">
         <v>35</v>
       </c>
       <c r="E41" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" t="s">
         <v>139</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>140</v>
-      </c>
-      <c r="C42" t="s">
-        <v>141</v>
       </c>
       <c r="D42">
         <v>57</v>
       </c>
       <c r="E42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>143</v>
       </c>
-      <c r="B43" t="s">
-        <v>144</v>
-      </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D43">
         <v>10.5</v>
       </c>
       <c r="E43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>146</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>147</v>
-      </c>
-      <c r="C45" t="s">
-        <v>148</v>
       </c>
       <c r="D45">
         <v>26.5</v>
       </c>
       <c r="E45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>150</v>
-      </c>
-      <c r="B46" t="s">
-        <v>151</v>
       </c>
       <c r="C46" t="s">
         <v>80</v>
@@ -1750,15 +1788,15 @@
         <v>124</v>
       </c>
       <c r="E46" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>153</v>
-      </c>
-      <c r="B47" t="s">
-        <v>154</v>
       </c>
       <c r="C47" t="s">
         <v>90</v>
@@ -1767,15 +1805,15 @@
         <v>31.5</v>
       </c>
       <c r="E47" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>156</v>
-      </c>
-      <c r="B48" t="s">
-        <v>157</v>
       </c>
       <c r="C48" t="s">
         <v>110</v>
@@ -1787,12 +1825,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" t="s">
         <v>158</v>
-      </c>
-      <c r="B49" t="s">
-        <v>159</v>
       </c>
       <c r="C49" t="s">
         <v>33</v>
@@ -1801,15 +1839,15 @@
         <v>18</v>
       </c>
       <c r="E49" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
         <v>161</v>
-      </c>
-      <c r="B50" t="s">
-        <v>162</v>
       </c>
       <c r="C50" t="s">
         <v>65</v>
@@ -1818,49 +1856,49 @@
         <v>46.5</v>
       </c>
       <c r="E50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>164</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>165</v>
-      </c>
-      <c r="C51" t="s">
-        <v>166</v>
       </c>
       <c r="D51">
         <v>47.25</v>
       </c>
       <c r="E51" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D52">
         <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" t="s">
         <v>168</v>
-      </c>
-      <c r="B53" t="s">
-        <v>169</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
@@ -1869,32 +1907,37 @@
         <v>24</v>
       </c>
       <c r="E53" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
         <v>171</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>172</v>
-      </c>
-      <c r="C54" t="s">
-        <v>173</v>
       </c>
       <c r="D54">
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" t="s">
         <v>174</v>
-      </c>
-      <c r="B56" t="s">
-        <v>175</v>
       </c>
       <c r="C56" t="s">
         <v>90</v>
@@ -1903,15 +1946,15 @@
         <v>10.5</v>
       </c>
       <c r="E56" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" t="s">
         <v>176</v>
-      </c>
-      <c r="B57" t="s">
-        <v>177</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
@@ -1920,66 +1963,66 @@
         <v>4</v>
       </c>
       <c r="E57" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>179</v>
-      </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C58" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D58">
         <v>13.25</v>
       </c>
       <c r="E58" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" t="s">
         <v>180</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>181</v>
-      </c>
-      <c r="C59" t="s">
-        <v>182</v>
       </c>
       <c r="D59">
         <v>18.5</v>
       </c>
       <c r="E59" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>184</v>
-      </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D60">
         <v>10.5</v>
       </c>
       <c r="E60" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" t="s">
         <v>185</v>
-      </c>
-      <c r="B61" t="s">
-        <v>186</v>
       </c>
       <c r="C61" t="s">
         <v>43</v>
@@ -1988,15 +2031,15 @@
         <v>30</v>
       </c>
       <c r="E61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B62" t="s">
         <v>188</v>
-      </c>
-      <c r="B62" t="s">
-        <v>189</v>
       </c>
       <c r="C62" t="s">
         <v>110</v>
@@ -2005,49 +2048,49 @@
         <v>5.25</v>
       </c>
       <c r="E62" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>189</v>
+      </c>
+      <c r="B63" t="s">
         <v>190</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>191</v>
-      </c>
-      <c r="C63" t="s">
-        <v>192</v>
       </c>
       <c r="D63">
         <v>10.5</v>
       </c>
       <c r="E63" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" t="s">
         <v>193</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>194</v>
-      </c>
-      <c r="C64" t="s">
-        <v>195</v>
       </c>
       <c r="D64">
         <v>13</v>
       </c>
       <c r="E64" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>195</v>
+      </c>
+      <c r="B65" t="s">
         <v>196</v>
-      </c>
-      <c r="B65" t="s">
-        <v>197</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
@@ -2056,15 +2099,20 @@
         <v>4.5</v>
       </c>
       <c r="E65" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>197</v>
+      </c>
+      <c r="B67" t="s">
         <v>198</v>
-      </c>
-      <c r="B67" t="s">
-        <v>199</v>
       </c>
       <c r="C67" t="s">
         <v>27</v>
@@ -2073,12 +2121,12 @@
         <v>21.75</v>
       </c>
       <c r="E67" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>201</v>
       </c>
       <c r="B68" t="s">
         <v>103</v>
@@ -2090,15 +2138,15 @@
         <v>45</v>
       </c>
       <c r="E68" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B69" t="s">
         <v>203</v>
-      </c>
-      <c r="B69" t="s">
-        <v>204</v>
       </c>
       <c r="C69" t="s">
         <v>17</v>
@@ -2107,46 +2155,46 @@
         <v>12</v>
       </c>
       <c r="E69" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B70" t="s">
         <v>206</v>
       </c>
-      <c r="B70" t="s">
-        <v>207</v>
-      </c>
       <c r="C70" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D70">
         <v>5</v>
       </c>
       <c r="E70" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>207</v>
+      </c>
+      <c r="B71" t="s">
+        <v>198</v>
+      </c>
+      <c r="C71" t="s">
         <v>208</v>
-      </c>
-      <c r="B71" t="s">
-        <v>199</v>
-      </c>
-      <c r="C71" t="s">
-        <v>209</v>
       </c>
       <c r="D71">
         <v>45</v>
       </c>
       <c r="E71" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B72" t="s">
         <v>109</v>
@@ -2161,29 +2209,29 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>210</v>
+      </c>
+      <c r="B73" t="s">
         <v>211</v>
       </c>
-      <c r="B73" t="s">
-        <v>212</v>
-      </c>
       <c r="C73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D73">
         <v>13.5</v>
       </c>
       <c r="E73" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B74" t="s">
         <v>214</v>
-      </c>
-      <c r="B74" t="s">
-        <v>215</v>
       </c>
       <c r="C74" t="s">
         <v>17</v>
@@ -2192,7 +2240,7 @@
         <v>16</v>
       </c>
       <c r="E74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2207,7 +2255,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2219,7 +2267,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>